<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@2049638e13ea75df9cf29ad059ca0a662f92b1dd 🚀
</commit_message>
<xml_diff>
--- a/2023/data.xlsx
+++ b/2023/data.xlsx
@@ -5362,7 +5362,7 @@
         </is>
       </c>
       <c r="R51" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S51" t="n">
         <v>0.1</v>
@@ -15346,7 +15346,7 @@
         </is>
       </c>
       <c r="R157" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S157" t="n">
         <v>0</v>
@@ -15385,7 +15385,7 @@
         <v>5000</v>
       </c>
       <c r="AE157" t="n">
-        <v>13333.33333333333</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="158">
@@ -22249,7 +22249,7 @@
         </is>
       </c>
       <c r="R230" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S230" t="n">
         <v>0.4</v>
@@ -22288,7 +22288,7 @@
         <v>4166.666666666667</v>
       </c>
       <c r="AE230" t="n">
-        <v>11111.11111111111</v>
+        <v>4166.666666666667</v>
       </c>
     </row>
     <row r="231">
@@ -27927,7 +27927,7 @@
         </is>
       </c>
       <c r="R290" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S290" t="n">
         <v>0.02</v>
@@ -27966,7 +27966,7 @@
         <v>7333.333333333333</v>
       </c>
       <c r="AE290" t="n">
-        <v>19555.55555555555</v>
+        <v>7333.333333333333</v>
       </c>
     </row>
     <row r="291">
@@ -29718,7 +29718,7 @@
         </is>
       </c>
       <c r="R309" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S309" t="n">
         <v>0.3</v>
@@ -29757,7 +29757,7 @@
         <v>7291.666666666667</v>
       </c>
       <c r="AE309" t="n">
-        <v>19444.44444444445</v>
+        <v>7291.666666666667</v>
       </c>
     </row>
     <row r="310">
@@ -32679,7 +32679,7 @@
         </is>
       </c>
       <c r="R340" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S340" t="n">
         <v>0.1</v>
@@ -32718,7 +32718,7 @@
         <v>5275</v>
       </c>
       <c r="AE340" t="n">
-        <v>14066.66666666667</v>
+        <v>5275</v>
       </c>
     </row>
     <row r="341">
@@ -38592,7 +38592,7 @@
         </is>
       </c>
       <c r="R402" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S402" t="n">
         <v>0.2</v>
@@ -38635,7 +38635,7 @@
         <v>5833.333333333333</v>
       </c>
       <c r="AE402" t="n">
-        <v>15555.55555555555</v>
+        <v>5833.333333333333</v>
       </c>
     </row>
     <row r="403">
@@ -60787,7 +60787,7 @@
         </is>
       </c>
       <c r="R635" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S635" t="n">
         <v>0.1</v>
@@ -60830,7 +60830,7 @@
         <v>6000</v>
       </c>
       <c r="AE635" t="n">
-        <v>16000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="636">
@@ -62214,7 +62214,7 @@
         </is>
       </c>
       <c r="R650" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="S650" t="n">
         <v>0</v>
@@ -62253,7 +62253,7 @@
         <v>4700</v>
       </c>
       <c r="AE650" t="n">
-        <v>470</v>
+        <v>4700</v>
       </c>
     </row>
     <row r="651">
@@ -66297,7 +66297,7 @@
         </is>
       </c>
       <c r="R693" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S693" t="n">
         <v>0.4</v>
@@ -66336,7 +66336,7 @@
         <v>4864.583333333333</v>
       </c>
       <c r="AE693" t="n">
-        <v>12972.22222222222</v>
+        <v>4864.583333333333</v>
       </c>
     </row>
     <row r="694">

</xml_diff>